<commit_message>
the controller method and the button for uploading a schedule, select with all the specialties added
</commit_message>
<xml_diff>
--- a/src/main/resources/download/Schedule_example.xlsx
+++ b/src/main/resources/download/Schedule_example.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11114"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3654F1FF-F99B-44F3-9063-9A7DBA4A31DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA3EFC0-7D59-7244-A1DF-A243175F5A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27520" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Аркуш1" sheetId="1" r:id="rId1"/>
@@ -1130,55 +1130,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1189,9 +1140,58 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1209,7 +1209,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Офіс">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1247,7 +1247,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Офіс">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1353,7 +1353,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Офіс">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1529,60 +1529,60 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="52.7109375" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="52.6640625" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.5" customWidth="1"/>
+    <col min="8" max="8" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="82" t="s">
+      <c r="C1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+    </row>
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="82" t="s">
+      <c r="C2" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-    </row>
-    <row r="3" spans="1:6" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+    </row>
+    <row r="3" spans="1:6" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="82"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C3" s="65"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+    </row>
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="84" t="s">
+      <c r="C4" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="83"/>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
-    </row>
-    <row r="5" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+    </row>
+    <row r="5" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="2"/>
@@ -1590,37 +1590,37 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="85" t="s">
+    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="77"/>
-      <c r="C6" s="77"/>
-      <c r="D6" s="77"/>
-      <c r="E6" s="77"/>
-      <c r="F6" s="77"/>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="76" t="s">
+      <c r="B6" s="69"/>
+      <c r="C6" s="69"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="69"/>
+    </row>
+    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="77"/>
-      <c r="C7" s="77"/>
-      <c r="D7" s="77"/>
-      <c r="E7" s="77"/>
-      <c r="F7" s="77"/>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="76" t="s">
+      <c r="B7" s="69"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
+    </row>
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="77"/>
-      <c r="C8" s="77"/>
-      <c r="D8" s="77"/>
-      <c r="E8" s="77"/>
-      <c r="F8" s="77"/>
-    </row>
-    <row r="9" spans="1:6" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="69"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="69"/>
+    </row>
+    <row r="9" spans="1:6" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4"/>
@@ -1628,7 +1628,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>55</v>
       </c>
@@ -1648,8 +1648,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="68" t="s">
+    <row r="11" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="71" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="16" t="s">
@@ -1668,9 +1668,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="66"/>
-      <c r="B12" s="80" t="s">
+    <row r="12" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="72"/>
+      <c r="B12" s="75" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="35" t="s">
@@ -1686,9 +1686,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="78"/>
-      <c r="B13" s="81"/>
+    <row r="13" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="73"/>
+      <c r="B13" s="76"/>
       <c r="C13" s="38" t="s">
         <v>39</v>
       </c>
@@ -1702,8 +1702,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="78"/>
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="73"/>
       <c r="B14" s="49" t="s">
         <v>7</v>
       </c>
@@ -1720,9 +1720,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="78"/>
-      <c r="B15" s="80" t="s">
+    <row r="15" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="73"/>
+      <c r="B15" s="75" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="35" t="s">
@@ -1738,9 +1738,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="78"/>
-      <c r="B16" s="81"/>
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="73"/>
+      <c r="B16" s="76"/>
       <c r="C16" s="35" t="s">
         <v>40</v>
       </c>
@@ -1754,9 +1754,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="78"/>
-      <c r="B17" s="80" t="s">
+    <row r="17" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="73"/>
+      <c r="B17" s="75" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="38" t="s">
@@ -1772,9 +1772,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="78"/>
-      <c r="B18" s="80"/>
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="73"/>
+      <c r="B18" s="75"/>
       <c r="C18" s="35" t="s">
         <v>40</v>
       </c>
@@ -1788,8 +1788,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="78"/>
+    <row r="19" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="73"/>
       <c r="B19" s="49" t="s">
         <v>17</v>
       </c>
@@ -1806,8 +1806,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="79"/>
+    <row r="20" spans="1:6" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="74"/>
       <c r="B20" s="51" t="s">
         <v>18</v>
       </c>
@@ -1816,8 +1816,8 @@
       <c r="E20" s="45"/>
       <c r="F20" s="46"/>
     </row>
-    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="68" t="s">
+    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="71" t="s">
         <v>11</v>
       </c>
       <c r="B21" s="14" t="s">
@@ -1836,9 +1836,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="66"/>
-      <c r="B22" s="70" t="s">
+    <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="72"/>
+      <c r="B22" s="77" t="s">
         <v>6</v>
       </c>
       <c r="C22" s="22" t="s">
@@ -1854,9 +1854,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="66"/>
-      <c r="B23" s="70"/>
+    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="72"/>
+      <c r="B23" s="77"/>
       <c r="C23" s="22" t="s">
         <v>34</v>
       </c>
@@ -1870,9 +1870,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="66"/>
-      <c r="B24" s="72"/>
+    <row r="24" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="72"/>
+      <c r="B24" s="81"/>
       <c r="C24" s="35" t="s">
         <v>38</v>
       </c>
@@ -1886,8 +1886,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="66"/>
+    <row r="25" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="72"/>
       <c r="B25" s="61" t="s">
         <v>7</v>
       </c>
@@ -1904,9 +1904,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="66"/>
-      <c r="B26" s="70" t="s">
+    <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="72"/>
+      <c r="B26" s="77" t="s">
         <v>8</v>
       </c>
       <c r="C26" s="22" t="s">
@@ -1922,9 +1922,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="66"/>
-      <c r="B27" s="70"/>
+    <row r="27" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A27" s="72"/>
+      <c r="B27" s="77"/>
       <c r="C27" s="22" t="s">
         <v>57</v>
       </c>
@@ -1938,9 +1938,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="66"/>
-      <c r="B28" s="70"/>
+    <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="72"/>
+      <c r="B28" s="77"/>
       <c r="C28" s="35" t="s">
         <v>38</v>
       </c>
@@ -1954,9 +1954,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="66"/>
-      <c r="B29" s="70" t="s">
+    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="72"/>
+      <c r="B29" s="77" t="s">
         <v>9</v>
       </c>
       <c r="C29" s="22" t="s">
@@ -1972,9 +1972,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="66"/>
-      <c r="B30" s="72"/>
+    <row r="30" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A30" s="72"/>
+      <c r="B30" s="81"/>
       <c r="C30" s="22" t="s">
         <v>57</v>
       </c>
@@ -1988,9 +1988,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="66"/>
-      <c r="B31" s="70" t="s">
+    <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="72"/>
+      <c r="B31" s="77" t="s">
         <v>17</v>
       </c>
       <c r="C31" s="22" t="s">
@@ -2006,9 +2006,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="66"/>
-      <c r="B32" s="70"/>
+    <row r="32" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A32" s="72"/>
+      <c r="B32" s="77"/>
       <c r="C32" s="22" t="s">
         <v>57</v>
       </c>
@@ -2022,8 +2022,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="69"/>
+    <row r="33" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="78"/>
       <c r="B33" s="48" t="s">
         <v>18</v>
       </c>
@@ -2040,11 +2040,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="68" t="s">
+    <row r="34" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="71" t="s">
+      <c r="B34" s="83" t="s">
         <v>5</v>
       </c>
       <c r="C34" s="19" t="s">
@@ -2060,9 +2060,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="66"/>
-      <c r="B35" s="72"/>
+    <row r="35" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="72"/>
+      <c r="B35" s="81"/>
       <c r="C35" s="17" t="s">
         <v>45</v>
       </c>
@@ -2076,9 +2076,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="73"/>
-      <c r="B36" s="70" t="s">
+    <row r="36" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="79"/>
+      <c r="B36" s="77" t="s">
         <v>6</v>
       </c>
       <c r="C36" s="22" t="s">
@@ -2094,9 +2094,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="73"/>
-      <c r="B37" s="70"/>
+    <row r="37" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="79"/>
+      <c r="B37" s="77"/>
       <c r="C37" s="17" t="s">
         <v>45</v>
       </c>
@@ -2110,9 +2110,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="73"/>
-      <c r="B38" s="70"/>
+    <row r="38" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="79"/>
+      <c r="B38" s="77"/>
       <c r="C38" s="17" t="s">
         <v>45</v>
       </c>
@@ -2126,9 +2126,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="73"/>
-      <c r="B39" s="70"/>
+    <row r="39" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="79"/>
+      <c r="B39" s="77"/>
       <c r="C39" s="22" t="s">
         <v>46</v>
       </c>
@@ -2142,9 +2142,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="73"/>
-      <c r="B40" s="70" t="s">
+    <row r="40" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A40" s="79"/>
+      <c r="B40" s="77" t="s">
         <v>7</v>
       </c>
       <c r="C40" s="56" t="s">
@@ -2160,9 +2160,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="73"/>
-      <c r="B41" s="70"/>
+    <row r="41" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A41" s="79"/>
+      <c r="B41" s="77"/>
       <c r="C41" s="22" t="s">
         <v>47</v>
       </c>
@@ -2176,9 +2176,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="73"/>
-      <c r="B42" s="70" t="s">
+    <row r="42" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A42" s="79"/>
+      <c r="B42" s="77" t="s">
         <v>8</v>
       </c>
       <c r="C42" s="56" t="s">
@@ -2194,9 +2194,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="73"/>
-      <c r="B43" s="70"/>
+    <row r="43" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A43" s="79"/>
+      <c r="B43" s="77"/>
       <c r="C43" s="22" t="s">
         <v>47</v>
       </c>
@@ -2210,9 +2210,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="73"/>
-      <c r="B44" s="70"/>
+    <row r="44" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A44" s="79"/>
+      <c r="B44" s="77"/>
       <c r="C44" s="18" t="s">
         <v>48</v>
       </c>
@@ -2226,9 +2226,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="73"/>
-      <c r="B45" s="70" t="s">
+    <row r="45" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A45" s="79"/>
+      <c r="B45" s="77" t="s">
         <v>9</v>
       </c>
       <c r="C45" s="22" t="s">
@@ -2244,9 +2244,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="73"/>
-      <c r="B46" s="70"/>
+    <row r="46" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A46" s="79"/>
+      <c r="B46" s="77"/>
       <c r="C46" s="56" t="s">
         <v>64</v>
       </c>
@@ -2260,9 +2260,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="73"/>
-      <c r="B47" s="72"/>
+    <row r="47" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A47" s="79"/>
+      <c r="B47" s="81"/>
       <c r="C47" s="18" t="s">
         <v>48</v>
       </c>
@@ -2276,9 +2276,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="73"/>
-      <c r="B48" s="70" t="s">
+    <row r="48" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A48" s="79"/>
+      <c r="B48" s="77" t="s">
         <v>17</v>
       </c>
       <c r="C48" s="22" t="s">
@@ -2294,9 +2294,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="73"/>
-      <c r="B49" s="70"/>
+    <row r="49" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A49" s="79"/>
+      <c r="B49" s="77"/>
       <c r="C49" s="56" t="s">
         <v>64</v>
       </c>
@@ -2310,9 +2310,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="73"/>
-      <c r="B50" s="70"/>
+    <row r="50" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A50" s="79"/>
+      <c r="B50" s="77"/>
       <c r="C50" s="22" t="s">
         <v>46</v>
       </c>
@@ -2326,9 +2326,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="73"/>
-      <c r="B51" s="72"/>
+    <row r="51" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A51" s="79"/>
+      <c r="B51" s="81"/>
       <c r="C51" s="18" t="s">
         <v>48</v>
       </c>
@@ -2342,9 +2342,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="73"/>
-      <c r="B52" s="70" t="s">
+    <row r="52" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A52" s="79"/>
+      <c r="B52" s="77" t="s">
         <v>18</v>
       </c>
       <c r="C52" s="56" t="s">
@@ -2360,9 +2360,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="73"/>
-      <c r="B53" s="70"/>
+    <row r="53" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A53" s="79"/>
+      <c r="B53" s="77"/>
       <c r="C53" s="56" t="s">
         <v>64</v>
       </c>
@@ -2376,9 +2376,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="73"/>
-      <c r="B54" s="70"/>
+    <row r="54" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A54" s="79"/>
+      <c r="B54" s="77"/>
       <c r="C54" s="56" t="s">
         <v>64</v>
       </c>
@@ -2392,9 +2392,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A55" s="73"/>
-      <c r="B55" s="70"/>
+    <row r="55" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A55" s="79"/>
+      <c r="B55" s="77"/>
       <c r="C55" s="56" t="s">
         <v>64</v>
       </c>
@@ -2408,9 +2408,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="74"/>
-      <c r="B56" s="75"/>
+    <row r="56" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="80"/>
+      <c r="B56" s="82"/>
       <c r="C56" s="56" t="s">
         <v>64</v>
       </c>
@@ -2424,8 +2424,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="68" t="s">
+    <row r="57" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="71" t="s">
         <v>13</v>
       </c>
       <c r="B57" s="14" t="s">
@@ -2436,8 +2436,8 @@
       <c r="E57" s="21"/>
       <c r="F57" s="55"/>
     </row>
-    <row r="58" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="66"/>
+    <row r="58" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="72"/>
       <c r="B58" s="47" t="s">
         <v>6</v>
       </c>
@@ -2454,9 +2454,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="66"/>
-      <c r="B59" s="70" t="s">
+    <row r="59" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="72"/>
+      <c r="B59" s="77" t="s">
         <v>7</v>
       </c>
       <c r="C59" s="5" t="s">
@@ -2472,9 +2472,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="66"/>
-      <c r="B60" s="72"/>
+    <row r="60" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="72"/>
+      <c r="B60" s="81"/>
       <c r="C60" s="22" t="s">
         <v>67</v>
       </c>
@@ -2488,9 +2488,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="66"/>
-      <c r="B61" s="70" t="s">
+    <row r="61" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="72"/>
+      <c r="B61" s="77" t="s">
         <v>8</v>
       </c>
       <c r="C61" s="22" t="s">
@@ -2506,9 +2506,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="66"/>
-      <c r="B62" s="70"/>
+    <row r="62" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="72"/>
+      <c r="B62" s="77"/>
       <c r="C62" s="5" t="s">
         <v>35</v>
       </c>
@@ -2522,9 +2522,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="66"/>
-      <c r="B63" s="70"/>
+    <row r="63" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="72"/>
+      <c r="B63" s="77"/>
       <c r="C63" s="56" t="s">
         <v>64</v>
       </c>
@@ -2538,9 +2538,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="66"/>
-      <c r="B64" s="70" t="s">
+    <row r="64" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="72"/>
+      <c r="B64" s="77" t="s">
         <v>9</v>
       </c>
       <c r="C64" s="56" t="s">
@@ -2556,9 +2556,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="66"/>
-      <c r="B65" s="70"/>
+    <row r="65" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="72"/>
+      <c r="B65" s="77"/>
       <c r="C65" s="5" t="s">
         <v>35</v>
       </c>
@@ -2572,8 +2572,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="66"/>
+    <row r="66" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="72"/>
       <c r="B66" s="53" t="s">
         <v>17</v>
       </c>
@@ -2590,8 +2590,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="69"/>
+    <row r="67" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="78"/>
       <c r="B67" s="48" t="s">
         <v>18</v>
       </c>
@@ -2600,11 +2600,11 @@
       <c r="E67" s="31"/>
       <c r="F67" s="41"/>
     </row>
-    <row r="68" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A68" s="68" t="s">
+    <row r="68" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A68" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="B68" s="71" t="s">
+      <c r="B68" s="83" t="s">
         <v>5</v>
       </c>
       <c r="C68" s="58" t="s">
@@ -2620,9 +2620,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A69" s="66"/>
-      <c r="B69" s="70"/>
+    <row r="69" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A69" s="72"/>
+      <c r="B69" s="77"/>
       <c r="C69" s="56" t="s">
         <v>36</v>
       </c>
@@ -2636,9 +2636,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A70" s="66"/>
-      <c r="B70" s="70"/>
+    <row r="70" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A70" s="72"/>
+      <c r="B70" s="77"/>
       <c r="C70" s="56" t="s">
         <v>36</v>
       </c>
@@ -2652,9 +2652,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A71" s="66"/>
-      <c r="B71" s="70"/>
+    <row r="71" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A71" s="72"/>
+      <c r="B71" s="77"/>
       <c r="C71" s="56" t="s">
         <v>36</v>
       </c>
@@ -2668,9 +2668,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A72" s="66"/>
-      <c r="B72" s="70"/>
+    <row r="72" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A72" s="72"/>
+      <c r="B72" s="77"/>
       <c r="C72" s="56" t="s">
         <v>36</v>
       </c>
@@ -2684,9 +2684,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A73" s="66"/>
-      <c r="B73" s="72"/>
+    <row r="73" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A73" s="72"/>
+      <c r="B73" s="81"/>
       <c r="C73" s="18" t="s">
         <v>42</v>
       </c>
@@ -2700,9 +2700,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A74" s="66"/>
-      <c r="B74" s="70" t="s">
+    <row r="74" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A74" s="72"/>
+      <c r="B74" s="77" t="s">
         <v>6</v>
       </c>
       <c r="C74" s="56" t="s">
@@ -2718,9 +2718,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A75" s="66"/>
-      <c r="B75" s="70"/>
+    <row r="75" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A75" s="72"/>
+      <c r="B75" s="77"/>
       <c r="C75" s="18" t="s">
         <v>42</v>
       </c>
@@ -2734,9 +2734,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A76" s="66"/>
-      <c r="B76" s="70"/>
+    <row r="76" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A76" s="72"/>
+      <c r="B76" s="77"/>
       <c r="C76" s="56" t="s">
         <v>36</v>
       </c>
@@ -2750,9 +2750,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A77" s="66"/>
-      <c r="B77" s="70" t="s">
+    <row r="77" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A77" s="72"/>
+      <c r="B77" s="77" t="s">
         <v>7</v>
       </c>
       <c r="C77" s="56" t="s">
@@ -2768,9 +2768,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A78" s="66"/>
-      <c r="B78" s="70"/>
+    <row r="78" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A78" s="72"/>
+      <c r="B78" s="77"/>
       <c r="C78" s="56" t="s">
         <v>59</v>
       </c>
@@ -2784,9 +2784,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A79" s="66"/>
-      <c r="B79" s="70"/>
+    <row r="79" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A79" s="72"/>
+      <c r="B79" s="77"/>
       <c r="C79" s="56" t="s">
         <v>36</v>
       </c>
@@ -2800,8 +2800,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A80" s="66"/>
+    <row r="80" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A80" s="72"/>
       <c r="B80" s="62" t="s">
         <v>8</v>
       </c>
@@ -2818,8 +2818,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A81" s="66"/>
+    <row r="81" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A81" s="72"/>
       <c r="B81" s="62" t="s">
         <v>9</v>
       </c>
@@ -2836,8 +2836,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A82" s="66"/>
+    <row r="82" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A82" s="72"/>
       <c r="B82" s="62" t="s">
         <v>17</v>
       </c>
@@ -2854,8 +2854,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="67"/>
+    <row r="83" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="85"/>
       <c r="B83" s="12" t="s">
         <v>18</v>
       </c>
@@ -2864,8 +2864,8 @@
       <c r="E83" s="63"/>
       <c r="F83" s="64"/>
     </row>
-    <row r="84" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A84" s="65" t="s">
+    <row r="84" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A84" s="84" t="s">
         <v>16</v>
       </c>
       <c r="B84" s="13" t="s">
@@ -2884,8 +2884,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A85" s="66"/>
+    <row r="85" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A85" s="72"/>
       <c r="B85" s="40" t="s">
         <v>6</v>
       </c>
@@ -2902,8 +2902,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="66"/>
+    <row r="86" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A86" s="72"/>
       <c r="B86" s="40" t="s">
         <v>7</v>
       </c>
@@ -2920,8 +2920,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A87" s="66"/>
+    <row r="87" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A87" s="72"/>
       <c r="B87" s="40" t="s">
         <v>8</v>
       </c>
@@ -2938,8 +2938,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A88" s="66"/>
+    <row r="88" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A88" s="72"/>
       <c r="B88" s="40" t="s">
         <v>9</v>
       </c>
@@ -2956,8 +2956,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="67"/>
+    <row r="89" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="85"/>
       <c r="B89" s="12" t="s">
         <v>17</v>
       </c>
@@ -2966,7 +2966,7 @@
       <c r="E89" s="44"/>
       <c r="F89" s="25"/>
     </row>
-    <row r="90" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -2974,7 +2974,7 @@
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
     </row>
-    <row r="91" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -2982,7 +2982,7 @@
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
     </row>
-    <row r="92" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -2990,7 +2990,7 @@
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
     </row>
-    <row r="93" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -2998,7 +2998,7 @@
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
     </row>
-    <row r="94" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -3006,7 +3006,7 @@
       <c r="E94" s="1"/>
       <c r="F94" s="1"/>
     </row>
-    <row r="95" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -3014,7 +3014,7 @@
       <c r="E95" s="1"/>
       <c r="F95" s="1"/>
     </row>
-    <row r="96" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -3022,7 +3022,7 @@
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
     </row>
-    <row r="97" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -3030,7 +3030,7 @@
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
     </row>
-    <row r="98" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -3038,7 +3038,7 @@
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
     </row>
-    <row r="99" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -3046,7 +3046,7 @@
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
     </row>
-    <row r="100" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -3054,7 +3054,7 @@
       <c r="E100" s="1"/>
       <c r="F100" s="1"/>
     </row>
-    <row r="101" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -3062,7 +3062,7 @@
       <c r="E101" s="1"/>
       <c r="F101" s="1"/>
     </row>
-    <row r="102" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -3070,7 +3070,7 @@
       <c r="E102" s="1"/>
       <c r="F102" s="1"/>
     </row>
-    <row r="103" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -3078,7 +3078,7 @@
       <c r="E103" s="1"/>
       <c r="F103" s="1"/>
     </row>
-    <row r="104" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -3086,7 +3086,7 @@
       <c r="E104" s="1"/>
       <c r="F104" s="1"/>
     </row>
-    <row r="105" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -3094,7 +3094,7 @@
       <c r="E105" s="1"/>
       <c r="F105" s="1"/>
     </row>
-    <row r="106" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -3102,7 +3102,7 @@
       <c r="E106" s="1"/>
       <c r="F106" s="1"/>
     </row>
-    <row r="107" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -3110,7 +3110,7 @@
       <c r="E107" s="1"/>
       <c r="F107" s="1"/>
     </row>
-    <row r="108" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -3118,7 +3118,7 @@
       <c r="E108" s="1"/>
       <c r="F108" s="1"/>
     </row>
-    <row r="109" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -3126,7 +3126,7 @@
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
     </row>
-    <row r="110" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -3134,7 +3134,7 @@
       <c r="E110" s="1"/>
       <c r="F110" s="1"/>
     </row>
-    <row r="111" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -3142,7 +3142,7 @@
       <c r="E111" s="1"/>
       <c r="F111" s="1"/>
     </row>
-    <row r="112" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -3150,7 +3150,7 @@
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
     </row>
-    <row r="113" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -3158,7 +3158,7 @@
       <c r="E113" s="1"/>
       <c r="F113" s="1"/>
     </row>
-    <row r="114" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -3166,7 +3166,7 @@
       <c r="E114" s="1"/>
       <c r="F114" s="1"/>
     </row>
-    <row r="115" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -3174,7 +3174,7 @@
       <c r="E115" s="1"/>
       <c r="F115" s="1"/>
     </row>
-    <row r="116" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -3182,7 +3182,7 @@
       <c r="E116" s="1"/>
       <c r="F116" s="1"/>
     </row>
-    <row r="117" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -3190,7 +3190,7 @@
       <c r="E117" s="1"/>
       <c r="F117" s="1"/>
     </row>
-    <row r="118" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -3198,7 +3198,7 @@
       <c r="E118" s="1"/>
       <c r="F118" s="1"/>
     </row>
-    <row r="119" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -3206,7 +3206,7 @@
       <c r="E119" s="1"/>
       <c r="F119" s="1"/>
     </row>
-    <row r="120" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -3214,7 +3214,7 @@
       <c r="E120" s="1"/>
       <c r="F120" s="1"/>
     </row>
-    <row r="121" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -3222,7 +3222,7 @@
       <c r="E121" s="1"/>
       <c r="F121" s="1"/>
     </row>
-    <row r="122" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -3230,7 +3230,7 @@
       <c r="E122" s="1"/>
       <c r="F122" s="1"/>
     </row>
-    <row r="123" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -3238,7 +3238,7 @@
       <c r="E123" s="1"/>
       <c r="F123" s="1"/>
     </row>
-    <row r="124" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -3246,7 +3246,7 @@
       <c r="E124" s="1"/>
       <c r="F124" s="1"/>
     </row>
-    <row r="125" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -3254,7 +3254,7 @@
       <c r="E125" s="1"/>
       <c r="F125" s="1"/>
     </row>
-    <row r="126" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -3262,7 +3262,7 @@
       <c r="E126" s="1"/>
       <c r="F126" s="1"/>
     </row>
-    <row r="127" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -3270,7 +3270,7 @@
       <c r="E127" s="1"/>
       <c r="F127" s="1"/>
     </row>
-    <row r="128" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -3278,7 +3278,7 @@
       <c r="E128" s="1"/>
       <c r="F128" s="1"/>
     </row>
-    <row r="129" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -3286,7 +3286,7 @@
       <c r="E129" s="1"/>
       <c r="F129" s="1"/>
     </row>
-    <row r="130" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -3294,7 +3294,7 @@
       <c r="E130" s="1"/>
       <c r="F130" s="1"/>
     </row>
-    <row r="131" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -3302,7 +3302,7 @@
       <c r="E131" s="1"/>
       <c r="F131" s="1"/>
     </row>
-    <row r="132" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -3310,7 +3310,7 @@
       <c r="E132" s="1"/>
       <c r="F132" s="1"/>
     </row>
-    <row r="133" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -3318,7 +3318,7 @@
       <c r="E133" s="1"/>
       <c r="F133" s="1"/>
     </row>
-    <row r="134" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -3326,7 +3326,7 @@
       <c r="E134" s="1"/>
       <c r="F134" s="1"/>
     </row>
-    <row r="135" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -3334,7 +3334,7 @@
       <c r="E135" s="1"/>
       <c r="F135" s="1"/>
     </row>
-    <row r="136" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -3342,7 +3342,7 @@
       <c r="E136" s="1"/>
       <c r="F136" s="1"/>
     </row>
-    <row r="137" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -3350,7 +3350,7 @@
       <c r="E137" s="1"/>
       <c r="F137" s="1"/>
     </row>
-    <row r="138" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -3358,7 +3358,7 @@
       <c r="E138" s="1"/>
       <c r="F138" s="1"/>
     </row>
-    <row r="139" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -3366,7 +3366,7 @@
       <c r="E139" s="1"/>
       <c r="F139" s="1"/>
     </row>
-    <row r="140" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -3374,7 +3374,7 @@
       <c r="E140" s="1"/>
       <c r="F140" s="1"/>
     </row>
-    <row r="141" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -3382,7 +3382,7 @@
       <c r="E141" s="1"/>
       <c r="F141" s="1"/>
     </row>
-    <row r="142" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -3390,7 +3390,7 @@
       <c r="E142" s="1"/>
       <c r="F142" s="1"/>
     </row>
-    <row r="143" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -3398,7 +3398,7 @@
       <c r="E143" s="1"/>
       <c r="F143" s="1"/>
     </row>
-    <row r="144" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -3406,7 +3406,7 @@
       <c r="E144" s="1"/>
       <c r="F144" s="1"/>
     </row>
-    <row r="145" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -3414,7 +3414,7 @@
       <c r="E145" s="1"/>
       <c r="F145" s="1"/>
     </row>
-    <row r="146" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -3422,7 +3422,7 @@
       <c r="E146" s="1"/>
       <c r="F146" s="1"/>
     </row>
-    <row r="147" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -3430,7 +3430,7 @@
       <c r="E147" s="1"/>
       <c r="F147" s="1"/>
     </row>
-    <row r="148" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -3438,7 +3438,7 @@
       <c r="E148" s="1"/>
       <c r="F148" s="1"/>
     </row>
-    <row r="149" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -3446,7 +3446,7 @@
       <c r="E149" s="1"/>
       <c r="F149" s="1"/>
     </row>
-    <row r="150" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -3454,7 +3454,7 @@
       <c r="E150" s="1"/>
       <c r="F150" s="1"/>
     </row>
-    <row r="151" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -3462,7 +3462,7 @@
       <c r="E151" s="1"/>
       <c r="F151" s="1"/>
     </row>
-    <row r="152" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -3470,7 +3470,7 @@
       <c r="E152" s="1"/>
       <c r="F152" s="1"/>
     </row>
-    <row r="153" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -3478,7 +3478,7 @@
       <c r="E153" s="1"/>
       <c r="F153" s="1"/>
     </row>
-    <row r="154" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -3486,7 +3486,7 @@
       <c r="E154" s="1"/>
       <c r="F154" s="1"/>
     </row>
-    <row r="155" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -3494,7 +3494,7 @@
       <c r="E155" s="1"/>
       <c r="F155" s="1"/>
     </row>
-    <row r="156" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -3502,7 +3502,7 @@
       <c r="E156" s="1"/>
       <c r="F156" s="1"/>
     </row>
-    <row r="157" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -3510,7 +3510,7 @@
       <c r="E157" s="1"/>
       <c r="F157" s="1"/>
     </row>
-    <row r="158" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -3518,7 +3518,7 @@
       <c r="E158" s="1"/>
       <c r="F158" s="1"/>
     </row>
-    <row r="159" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -3526,7 +3526,7 @@
       <c r="E159" s="1"/>
       <c r="F159" s="1"/>
     </row>
-    <row r="160" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -3534,7 +3534,7 @@
       <c r="E160" s="1"/>
       <c r="F160" s="1"/>
     </row>
-    <row r="161" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -3542,7 +3542,7 @@
       <c r="E161" s="1"/>
       <c r="F161" s="1"/>
     </row>
-    <row r="162" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -3550,7 +3550,7 @@
       <c r="E162" s="1"/>
       <c r="F162" s="1"/>
     </row>
-    <row r="163" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -3558,7 +3558,7 @@
       <c r="E163" s="1"/>
       <c r="F163" s="1"/>
     </row>
-    <row r="164" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -3566,7 +3566,7 @@
       <c r="E164" s="1"/>
       <c r="F164" s="1"/>
     </row>
-    <row r="165" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -3574,7 +3574,7 @@
       <c r="E165" s="1"/>
       <c r="F165" s="1"/>
     </row>
-    <row r="166" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -3582,7 +3582,7 @@
       <c r="E166" s="1"/>
       <c r="F166" s="1"/>
     </row>
-    <row r="167" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -3590,7 +3590,7 @@
       <c r="E167" s="1"/>
       <c r="F167" s="1"/>
     </row>
-    <row r="168" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -3598,7 +3598,7 @@
       <c r="E168" s="1"/>
       <c r="F168" s="1"/>
     </row>
-    <row r="169" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -3606,7 +3606,7 @@
       <c r="E169" s="1"/>
       <c r="F169" s="1"/>
     </row>
-    <row r="170" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -3614,7 +3614,7 @@
       <c r="E170" s="1"/>
       <c r="F170" s="1"/>
     </row>
-    <row r="171" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -3622,7 +3622,7 @@
       <c r="E171" s="1"/>
       <c r="F171" s="1"/>
     </row>
-    <row r="172" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -3630,7 +3630,7 @@
       <c r="E172" s="1"/>
       <c r="F172" s="1"/>
     </row>
-    <row r="173" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -3638,7 +3638,7 @@
       <c r="E173" s="1"/>
       <c r="F173" s="1"/>
     </row>
-    <row r="174" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -3646,7 +3646,7 @@
       <c r="E174" s="1"/>
       <c r="F174" s="1"/>
     </row>
-    <row r="175" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -3654,7 +3654,7 @@
       <c r="E175" s="1"/>
       <c r="F175" s="1"/>
     </row>
-    <row r="176" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -3662,7 +3662,7 @@
       <c r="E176" s="1"/>
       <c r="F176" s="1"/>
     </row>
-    <row r="177" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -3670,7 +3670,7 @@
       <c r="E177" s="1"/>
       <c r="F177" s="1"/>
     </row>
-    <row r="178" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -3678,7 +3678,7 @@
       <c r="E178" s="1"/>
       <c r="F178" s="1"/>
     </row>
-    <row r="179" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -3686,7 +3686,7 @@
       <c r="E179" s="1"/>
       <c r="F179" s="1"/>
     </row>
-    <row r="180" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -3694,7 +3694,7 @@
       <c r="E180" s="1"/>
       <c r="F180" s="1"/>
     </row>
-    <row r="181" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -3702,7 +3702,7 @@
       <c r="E181" s="1"/>
       <c r="F181" s="1"/>
     </row>
-    <row r="182" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -3710,7 +3710,7 @@
       <c r="E182" s="1"/>
       <c r="F182" s="1"/>
     </row>
-    <row r="183" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -3718,7 +3718,7 @@
       <c r="E183" s="1"/>
       <c r="F183" s="1"/>
     </row>
-    <row r="184" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -3726,7 +3726,7 @@
       <c r="E184" s="1"/>
       <c r="F184" s="1"/>
     </row>
-    <row r="185" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -3734,7 +3734,7 @@
       <c r="E185" s="1"/>
       <c r="F185" s="1"/>
     </row>
-    <row r="186" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -3742,7 +3742,7 @@
       <c r="E186" s="1"/>
       <c r="F186" s="1"/>
     </row>
-    <row r="187" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -3750,7 +3750,7 @@
       <c r="E187" s="1"/>
       <c r="F187" s="1"/>
     </row>
-    <row r="188" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -3758,7 +3758,7 @@
       <c r="E188" s="1"/>
       <c r="F188" s="1"/>
     </row>
-    <row r="189" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -3766,7 +3766,7 @@
       <c r="E189" s="1"/>
       <c r="F189" s="1"/>
     </row>
-    <row r="190" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -3774,7 +3774,7 @@
       <c r="E190" s="1"/>
       <c r="F190" s="1"/>
     </row>
-    <row r="191" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -3782,7 +3782,7 @@
       <c r="E191" s="1"/>
       <c r="F191" s="1"/>
     </row>
-    <row r="192" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -3790,7 +3790,7 @@
       <c r="E192" s="1"/>
       <c r="F192" s="1"/>
     </row>
-    <row r="193" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -3798,7 +3798,7 @@
       <c r="E193" s="1"/>
       <c r="F193" s="1"/>
     </row>
-    <row r="194" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
@@ -3806,7 +3806,7 @@
       <c r="E194" s="1"/>
       <c r="F194" s="1"/>
     </row>
-    <row r="195" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -3814,7 +3814,7 @@
       <c r="E195" s="1"/>
       <c r="F195" s="1"/>
     </row>
-    <row r="196" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
@@ -3822,7 +3822,7 @@
       <c r="E196" s="1"/>
       <c r="F196" s="1"/>
     </row>
-    <row r="197" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A197" s="1"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
@@ -3830,7 +3830,7 @@
       <c r="E197" s="1"/>
       <c r="F197" s="1"/>
     </row>
-    <row r="198" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A198" s="1"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
@@ -3838,7 +3838,7 @@
       <c r="E198" s="1"/>
       <c r="F198" s="1"/>
     </row>
-    <row r="199" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A199" s="1"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
@@ -3846,7 +3846,7 @@
       <c r="E199" s="1"/>
       <c r="F199" s="1"/>
     </row>
-    <row r="200" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A200" s="1"/>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
@@ -3854,7 +3854,7 @@
       <c r="E200" s="1"/>
       <c r="F200" s="1"/>
     </row>
-    <row r="201" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A201" s="1"/>
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
@@ -3862,7 +3862,7 @@
       <c r="E201" s="1"/>
       <c r="F201" s="1"/>
     </row>
-    <row r="202" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A202" s="1"/>
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
@@ -3870,7 +3870,7 @@
       <c r="E202" s="1"/>
       <c r="F202" s="1"/>
     </row>
-    <row r="203" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A203" s="1"/>
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
@@ -3878,7 +3878,7 @@
       <c r="E203" s="1"/>
       <c r="F203" s="1"/>
     </row>
-    <row r="204" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A204" s="1"/>
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
@@ -3886,7 +3886,7 @@
       <c r="E204" s="1"/>
       <c r="F204" s="1"/>
     </row>
-    <row r="205" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A205" s="1"/>
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
@@ -3894,7 +3894,7 @@
       <c r="E205" s="1"/>
       <c r="F205" s="1"/>
     </row>
-    <row r="206" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A206" s="1"/>
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
@@ -3902,7 +3902,7 @@
       <c r="E206" s="1"/>
       <c r="F206" s="1"/>
     </row>
-    <row r="207" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A207" s="1"/>
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
@@ -3910,7 +3910,7 @@
       <c r="E207" s="1"/>
       <c r="F207" s="1"/>
     </row>
-    <row r="208" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A208" s="1"/>
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
@@ -3918,7 +3918,7 @@
       <c r="E208" s="1"/>
       <c r="F208" s="1"/>
     </row>
-    <row r="209" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A209" s="1"/>
       <c r="B209" s="1"/>
       <c r="C209" s="1"/>
@@ -3926,7 +3926,7 @@
       <c r="E209" s="1"/>
       <c r="F209" s="1"/>
     </row>
-    <row r="210" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A210" s="1"/>
       <c r="B210" s="1"/>
       <c r="C210" s="1"/>
@@ -3934,7 +3934,7 @@
       <c r="E210" s="1"/>
       <c r="F210" s="1"/>
     </row>
-    <row r="211" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A211" s="1"/>
       <c r="B211" s="1"/>
       <c r="C211" s="1"/>
@@ -3942,7 +3942,7 @@
       <c r="E211" s="1"/>
       <c r="F211" s="1"/>
     </row>
-    <row r="212" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A212" s="1"/>
       <c r="B212" s="1"/>
       <c r="C212" s="1"/>
@@ -3950,7 +3950,7 @@
       <c r="E212" s="1"/>
       <c r="F212" s="1"/>
     </row>
-    <row r="213" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A213" s="1"/>
       <c r="B213" s="1"/>
       <c r="C213" s="1"/>
@@ -3958,7 +3958,7 @@
       <c r="E213" s="1"/>
       <c r="F213" s="1"/>
     </row>
-    <row r="214" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A214" s="1"/>
       <c r="B214" s="1"/>
       <c r="C214" s="1"/>
@@ -3966,7 +3966,7 @@
       <c r="E214" s="1"/>
       <c r="F214" s="1"/>
     </row>
-    <row r="215" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A215" s="1"/>
       <c r="B215" s="1"/>
       <c r="C215" s="1"/>
@@ -3976,17 +3976,15 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A11:A20"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="A84:A89"/>
+    <mergeCell ref="A68:A83"/>
+    <mergeCell ref="A57:A67"/>
+    <mergeCell ref="B74:B76"/>
+    <mergeCell ref="B68:B73"/>
+    <mergeCell ref="B77:B79"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="B64:B65"/>
     <mergeCell ref="B31:B32"/>
     <mergeCell ref="A21:A33"/>
     <mergeCell ref="B40:B41"/>
@@ -4000,15 +3998,17 @@
     <mergeCell ref="B52:B56"/>
     <mergeCell ref="B34:B35"/>
     <mergeCell ref="B48:B51"/>
-    <mergeCell ref="A84:A89"/>
-    <mergeCell ref="A68:A83"/>
-    <mergeCell ref="A57:A67"/>
-    <mergeCell ref="B74:B76"/>
-    <mergeCell ref="B68:B73"/>
-    <mergeCell ref="B77:B79"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A11:A20"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="A6:F6"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4021,7 +4021,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4034,7 +4034,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>